<commit_message>
update charts & readme
</commit_message>
<xml_diff>
--- a/readme_files/bootloader_summary.xlsx
+++ b/readme_files/bootloader_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2839FDEF-32DC-420D-9BF6-05A8D398408E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AC6104-58D1-4559-A6CC-18938B5E1A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="1050" windowWidth="21600" windowHeight="14175" activeTab="1" xr2:uid="{6C55A1A0-E8E8-4669-A1BD-2E037FD69E57}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="105">
   <si>
     <t>bootloader_platformio</t>
   </si>
@@ -333,9 +333,6 @@
     <t>notes</t>
   </si>
   <si>
-    <t>SPI_F407_based-on-fatfs-stm32-master</t>
-  </si>
-  <si>
     <t>has exFAT support</t>
   </si>
   <si>
@@ -343,6 +340,12 @@
   </si>
   <si>
     <t>SDIO_F746_STM32cube</t>
+  </si>
+  <si>
+    <t>SPI_F407ZG_based-on-fatfs-stm32-master</t>
+  </si>
+  <si>
+    <t>SDIO_F407VE_fatfs-stm32-master</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1363,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1528,45 +1531,45 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="14">
         <v>8004000</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="14">
         <v>8004000</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1587,7 +1590,7 @@
         <v>38</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.45">
@@ -1607,7 +1610,7 @@
         <v>60</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.45">
@@ -1627,7 +1630,7 @@
         <v>67</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.45">
@@ -1647,7 +1650,7 @@
         <v>75</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
@@ -1673,20 +1676,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="20" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="14">
         <v>8004000</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1695,7 +1698,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>94</v>
@@ -1707,7 +1710,7 @@
         <v>38</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
@@ -1744,7 +1747,7 @@
         <v>60</v>
       </c>
       <c r="H23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
update READ_ME, reduce image size to under 0x4000
</commit_message>
<xml_diff>
--- a/readme_files/bootloader_summary.xlsx
+++ b/readme_files/bootloader_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobku\Documents\GitHub\bootloader_SPI\readme_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D837E3C-B2AB-4BEA-8B87-AE9616FF3F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124CF25C-48E9-4142-BE06-CC32220FF77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2498" yWindow="997" windowWidth="21600" windowHeight="14175" activeTab="1" xr2:uid="{6C55A1A0-E8E8-4669-A1BD-2E037FD69E57}"/>
+    <workbookView xWindow="338" yWindow="1267" windowWidth="21600" windowHeight="14175" activeTab="1" xr2:uid="{6C55A1A0-E8E8-4669-A1BD-2E037FD69E57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,16 +354,16 @@
     <t>Cohesion3D Remixed</t>
   </si>
   <si>
-    <t>5E1C</t>
-  </si>
-  <si>
     <t>SPI_LPC1769_based-on-fatfs-stm32-master</t>
   </si>
   <si>
-    <t>Marlin default load is at 4000 so this bootloader is too big</t>
-  </si>
-  <si>
-    <t>0006000</t>
+    <t>3F44</t>
+  </si>
+  <si>
+    <t>0004000</t>
+  </si>
+  <si>
+    <t>Marlin default load is at 4000</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1384,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1694,24 +1694,24 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>107</v>
-      </c>
       <c r="D18" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>105</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">

</xml_diff>